<commit_message>
Updates to ICER calculation
</commit_message>
<xml_diff>
--- a/data-raw/01_public_parameters.xlsx
+++ b/data-raw/01_public_parameters.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27904"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PACER\PREDiCT\PREDiCT_e\PartSA Model\PartSA_repHTA\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\CRCFILE12\gcupples\PREDiCT\PartSA_repHTA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B808DE77A3F5A9D781095B350AD65C4E172367A4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C667E983-D7D1-4230-9C65-2EFF41F85889}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="871"/>
   </bookViews>
   <sheets>
     <sheet name="Workspace" sheetId="19" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <sheet name="3.5_TrialWeights" sheetId="9" r:id="rId12"/>
     <sheet name="3.6_TTOT" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -336,8 +335,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -445,7 +444,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -790,19 +789,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -810,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -818,7 +817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -827,7 +826,7 @@
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -835,7 +834,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -843,7 +842,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -851,7 +850,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -859,7 +858,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -875,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -883,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -898,14 +897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
@@ -917,7 +916,7 @@
     <col min="1023" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -967,7 +966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1117,7 +1116,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1217,7 +1216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1317,7 +1316,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1424,20 +1423,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -1448,7 +1447,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1475,7 +1474,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +1522,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1569,14 +1568,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1584,7 +1583,7 @@
     <col min="5" max="6" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1607,7 +1606,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1616,7 +1615,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1641,7 +1640,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1665,7 +1664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1680,20 +1679,20 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -1753,19 +1752,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1800,14 +1799,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -1817,7 +1816,7 @@
     <col min="1022" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1867,7 +1866,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1875,18 +1874,18 @@
         <v>25</v>
       </c>
       <c r="C3" s="8">
-        <v>139.41999999999999</v>
+        <v>127.23357437878371</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3">
         <f>C3*0.8</f>
-        <v>111.536</v>
+        <v>101.78685950302697</v>
       </c>
       <c r="F3">
         <f>C3*1.2</f>
-        <v>167.30399999999997</v>
+        <v>152.68028925454044</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -1895,7 +1894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1903,18 +1902,18 @@
         <v>25</v>
       </c>
       <c r="C4" s="8">
-        <v>104.86</v>
+        <v>95.69281677470633</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
       <c r="E4">
         <f>C4*0.8</f>
-        <v>83.888000000000005</v>
+        <v>76.554253419765061</v>
       </c>
       <c r="F4">
         <f>C4*1.2</f>
-        <v>125.83199999999999</v>
+        <v>114.8313801296476</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1923,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1931,18 +1930,18 @@
         <v>25</v>
       </c>
       <c r="C5" s="8">
-        <v>133.49</v>
+        <v>121.81946136426386</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5">
         <f>C5*0.8</f>
-        <v>106.79200000000002</v>
+        <v>97.455569091411093</v>
       </c>
       <c r="F5">
         <f>C5*1.2</f>
-        <v>160.18800000000002</v>
+        <v>146.18335363711662</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1951,7 +1950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1959,18 +1958,18 @@
         <v>35</v>
       </c>
       <c r="C6" s="8">
-        <v>1494.01</v>
+        <v>1363.4406977269464</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
       <c r="E6">
         <f>C6*0.8</f>
-        <v>1195.2080000000001</v>
+        <v>1090.7525581815571</v>
       </c>
       <c r="F6">
         <f>C6*1.2</f>
-        <v>1792.8119999999999</v>
+        <v>1636.1288372723357</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1979,7 +1978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
@@ -2013,12 +2012,14 @@
         <v>25</v>
       </c>
       <c r="C8">
+        <f>2002</f>
         <v>2002</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
       <c r="E8">
+        <f>C8</f>
         <v>2002</v>
       </c>
       <c r="F8" t="s">
@@ -2031,7 +2032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -2039,18 +2040,18 @@
         <v>35</v>
       </c>
       <c r="C9" s="8">
-        <v>1494.01</v>
+        <v>1363.4406977269464</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="E9">
         <f>C9*0.8</f>
-        <v>1195.2080000000001</v>
+        <v>1090.7525581815571</v>
       </c>
       <c r="F9">
         <f>C9*1.2</f>
-        <v>1792.8119999999999</v>
+        <v>1636.1288372723357</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
@@ -2059,7 +2060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -2083,7 +2084,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -2109,10 +2110,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
   </sheetData>
@@ -2122,14 +2123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
@@ -2137,7 +2138,7 @@
     <col min="1022" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2210,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2367,14 +2368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
@@ -2383,7 +2384,7 @@
     <col min="1022" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2454,7 +2455,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2479,7 +2480,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2503,7 +2504,7 @@
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2527,7 +2528,7 @@
       </c>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2552,7 +2553,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2579,7 +2580,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2603,17 +2604,17 @@
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
+  <sortState ref="A2:G9">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2622,20 +2623,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -2658,23 +2659,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
       <c r="B2">
-        <v>139.01</v>
+        <v>126.86521516588937</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2">
         <f>B2*0.8</f>
-        <v>111.208</v>
+        <v>101.4921721327115</v>
       </c>
       <c r="E2">
         <f>B2*1.2</f>
-        <v>166.81199999999998</v>
+        <v>152.23825819906725</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -2683,23 +2684,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
       <c r="B3">
-        <v>116.94</v>
+        <v>106.72057071073046</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" si="0">B3*0.8</f>
-        <v>93.552000000000007</v>
+        <v>85.376456568584373</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E9" si="1">B3*1.2</f>
-        <v>140.328</v>
+        <v>128.06468485287655</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -2708,7 +2709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2733,23 +2734,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5">
-        <v>142.52000000000001</v>
+        <v>130.06917290304321</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>114.01600000000002</v>
+        <v>104.05533832243458</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>171.024</v>
+        <v>156.08300748365184</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -2758,23 +2759,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
       <c r="B6">
-        <v>183.3</v>
+        <v>167.28496463077394</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>146.64000000000001</v>
+        <v>133.82797170461916</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>219.96</v>
+        <v>200.74195755692872</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
@@ -2783,23 +2784,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7">
-        <v>139.46</v>
+        <v>127.27194513012687</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>111.56800000000001</v>
+        <v>101.8175561041015</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>167.352</v>
+        <v>152.72633415615223</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2808,7 +2809,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2833,23 +2834,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
       <c r="B9">
-        <v>3.07</v>
+        <v>2.8010648480506681</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>2.456</v>
+        <v>2.2408518784405347</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>3.6839999999999997</v>
+        <v>3.3612778176608016</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -2864,21 +2865,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2948,7 +2949,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2970,7 +2971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -3014,7 +3015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -3102,7 +3103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -3190,7 +3191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3219,14 +3220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
@@ -3234,7 +3235,7 @@
     <col min="1022" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3257,7 +3258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -3299,7 +3300,7 @@
         <v>0.86680000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>0.70620000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -3337,7 +3338,7 @@
         <v>0.86680000000000013</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -3363,14 +3364,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
@@ -3379,7 +3380,7 @@
     <col min="1023" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -3645,7 +3646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Packages updated. Added plot files
</commit_message>
<xml_diff>
--- a/data-raw/01_public_parameters.xlsx
+++ b/data-raw/01_public_parameters.xlsx
@@ -793,7 +793,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1803,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,18 +1874,18 @@
         <v>25</v>
       </c>
       <c r="C3" s="8">
-        <v>127.23357437878371</v>
+        <v>139.41999999999999</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3">
         <f>C3*0.8</f>
-        <v>101.78685950302697</v>
+        <v>111.536</v>
       </c>
       <c r="F3">
         <f>C3*1.2</f>
-        <v>152.68028925454044</v>
+        <v>167.30399999999997</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -1902,18 +1902,18 @@
         <v>25</v>
       </c>
       <c r="C4" s="8">
-        <v>95.69281677470633</v>
+        <v>104.86</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
       <c r="E4">
         <f>C4*0.8</f>
-        <v>76.554253419765061</v>
+        <v>83.888000000000005</v>
       </c>
       <c r="F4">
         <f>C4*1.2</f>
-        <v>114.8313801296476</v>
+        <v>125.83199999999999</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1930,18 +1930,18 @@
         <v>25</v>
       </c>
       <c r="C5" s="8">
-        <v>121.81946136426386</v>
+        <v>133.49</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5">
         <f>C5*0.8</f>
-        <v>97.455569091411093</v>
+        <v>106.79200000000002</v>
       </c>
       <c r="F5">
         <f>C5*1.2</f>
-        <v>146.18335363711662</v>
+        <v>160.18800000000002</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1958,18 +1958,18 @@
         <v>35</v>
       </c>
       <c r="C6" s="8">
-        <v>1363.4406977269464</v>
+        <v>1494.01</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
       <c r="E6">
         <f>C6*0.8</f>
-        <v>1090.7525581815571</v>
+        <v>1195.2080000000001</v>
       </c>
       <c r="F6">
         <f>C6*1.2</f>
-        <v>1636.1288372723357</v>
+        <v>1792.8119999999999</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -2012,14 +2012,12 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <f>2002</f>
         <v>2002</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
       <c r="E8">
-        <f>C8</f>
         <v>2002</v>
       </c>
       <c r="F8" t="s">
@@ -2040,18 +2038,18 @@
         <v>35</v>
       </c>
       <c r="C9" s="8">
-        <v>1363.4406977269464</v>
+        <v>1494.01</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="E9">
         <f>C9*0.8</f>
-        <v>1090.7525581815571</v>
+        <v>1195.2080000000001</v>
       </c>
       <c r="F9">
         <f>C9*1.2</f>
-        <v>1636.1288372723357</v>
+        <v>1792.8119999999999</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
@@ -2372,7 +2370,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +2625,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,18 +2662,18 @@
         <v>45</v>
       </c>
       <c r="B2">
-        <v>126.86521516588937</v>
+        <v>139.01</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2">
         <f>B2*0.8</f>
-        <v>101.4921721327115</v>
+        <v>111.208</v>
       </c>
       <c r="E2">
         <f>B2*1.2</f>
-        <v>152.23825819906725</v>
+        <v>166.81199999999998</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -2689,18 +2687,18 @@
         <v>47</v>
       </c>
       <c r="B3">
-        <v>106.72057071073046</v>
+        <v>116.94</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" si="0">B3*0.8</f>
-        <v>85.376456568584373</v>
+        <v>93.552000000000007</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E9" si="1">B3*1.2</f>
-        <v>128.06468485287655</v>
+        <v>140.328</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -2739,18 +2737,18 @@
         <v>49</v>
       </c>
       <c r="B5">
-        <v>130.06917290304321</v>
+        <v>142.52000000000001</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>104.05533832243458</v>
+        <v>114.01600000000002</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>156.08300748365184</v>
+        <v>171.024</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -2764,18 +2762,18 @@
         <v>51</v>
       </c>
       <c r="B6">
-        <v>167.28496463077394</v>
+        <v>183.3</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>133.82797170461916</v>
+        <v>146.64000000000001</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>200.74195755692872</v>
+        <v>219.96</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
@@ -2789,18 +2787,18 @@
         <v>52</v>
       </c>
       <c r="B7">
-        <v>127.27194513012687</v>
+        <v>139.46</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>101.8175561041015</v>
+        <v>111.56800000000001</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>152.72633415615223</v>
+        <v>167.352</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2839,18 +2837,18 @@
         <v>50</v>
       </c>
       <c r="B9">
-        <v>2.8010648480506681</v>
+        <v>3.07</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>2.2408518784405347</v>
+        <v>2.456</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>3.3612778176608016</v>
+        <v>3.6839999999999997</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -3224,7 +3222,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>